<commit_message>
Animation working Conflict detection in progress
</commit_message>
<xml_diff>
--- a/rawdata/Segments.xlsx
+++ b/rawdata/Segments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holly\Desktop\rail_simulator\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA4777-867D-42A5-BB77-8D0A610B9B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B521A87F-4864-4A9C-A3A6-C03F68BD2CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{9BAFB3FB-CF0E-41D0-A3EB-B7AAE1AD5716}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9BAFB3FB-CF0E-41D0-A3EB-B7AAE1AD5716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>To</t>
   </si>
   <si>
-    <t>Line</t>
-  </si>
-  <si>
     <t>Distance</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>To Milepost</t>
+  </si>
+  <si>
+    <t>Track</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,39 +504,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>220077</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>209617</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>10460</v>
@@ -547,19 +547,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>209617</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>197546</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>12071</v>
@@ -570,19 +570,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>197546</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>175418</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>22128</v>
@@ -593,19 +593,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>175418</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>161739</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5">
         <v>13679</v>
@@ -616,19 +616,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>161739</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>161336.33499999999</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <v>402.66500000000002</v>
@@ -639,19 +639,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>161336.33499999999</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>144261</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <v>17075.334999999999</v>
@@ -662,19 +662,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>144261</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>126558</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8">
         <v>17703</v>
@@ -685,19 +685,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>126558</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>113056</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9">
         <v>13502</v>
@@ -708,19 +708,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>113056</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>84716</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10">
         <v>28340</v>
@@ -731,19 +731,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>84716</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>70006</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <v>14710</v>
@@ -754,19 +754,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>70006</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>46269</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <v>23737</v>
@@ -777,19 +777,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>46269</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13">
         <v>35003</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <v>11266</v>
@@ -800,19 +800,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>35003</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>28163</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14">
         <v>6840</v>
@@ -823,94 +823,94 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>28163</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15">
         <v>22128</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15">
         <v>6035</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>22128</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16">
         <v>4426</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16">
         <v>17702</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>4426</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17">
         <v>1600</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17">
         <v>2826</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>1600</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18">
         <v>1600</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>